<commit_message>
Commit after change to quarto version, but before change to new raw limits version of TOST
Anaysis_01.R works, but refined further in quarto version
</commit_message>
<xml_diff>
--- a/data/results.xlsx
+++ b/data/results.xlsx
@@ -359,7 +359,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="1" sqref="B:B A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -570,7 +570,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fiddled with TOST printing & added LC to results
</commit_message>
<xml_diff>
--- a/data/results.xlsx
+++ b/data/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="lcdod" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,12 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t xml:space="preserve">cushion</t>
   </si>
   <si>
     <t xml:space="preserve">foam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LC</t>
   </si>
   <si>
     <t xml:space="preserve">L135</t>
@@ -86,7 +89,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5">
@@ -356,10 +359,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="1" sqref="B:B A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -380,174 +383,207 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>53.4633333333333</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="4" t="n">
+        <v>53.4633333333333</v>
+      </c>
+      <c r="E2" s="5" t="n">
         <v>7.21333333333334</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="F2" s="4" t="n">
         <v>13.4566666666667</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>50.53</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="4" t="n">
+        <v>50.53</v>
+      </c>
+      <c r="E3" s="5" t="n">
         <v>7.90333333333334</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="F3" s="4" t="n">
         <v>14.81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>46.2033333333333</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="4" t="n">
+        <v>46.2033333333333</v>
+      </c>
+      <c r="E4" s="5" t="n">
         <v>7.17666666666667</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="F4" s="4" t="n">
         <v>14.2566666666667</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>45.9466666666667</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="4" t="n">
+        <v>45.9466666666667</v>
+      </c>
+      <c r="E5" s="5" t="n">
         <v>7.01666666666667</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="F5" s="4" t="n">
         <v>13.9466666666667</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>52.3566666666667</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="4" t="n">
+        <v>52.3566666666667</v>
+      </c>
+      <c r="E6" s="5" t="n">
         <v>7.60000000000001</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="F6" s="4" t="n">
         <v>14.04</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>43.7533333333333</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="4" t="n">
+        <v>43.7533333333333</v>
+      </c>
+      <c r="E7" s="5" t="n">
         <v>7.48</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="F7" s="4" t="n">
         <v>15.26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>44.5766666666667</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="4" t="n">
+        <v>44.5766666666667</v>
+      </c>
+      <c r="E8" s="5" t="n">
         <v>7.38000000000001</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="F8" s="4" t="n">
         <v>14.4666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>44.8333333333333</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="4" t="n">
+        <v>44.8333333333333</v>
+      </c>
+      <c r="E9" s="5" t="n">
         <v>7.53333333333333</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="F9" s="4" t="n">
         <v>15.1633333333333</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>43.9833333333333</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="4" t="n">
+        <v>43.9833333333333</v>
+      </c>
+      <c r="E10" s="5" t="n">
         <v>7.36000000000001</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="F10" s="4" t="n">
         <v>14.9266666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="9" t="n">
         <v>43.86</v>
       </c>
-      <c r="D11" s="10" t="n">
+      <c r="D11" s="9" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="E11" s="10" t="n">
         <v>7.05333333333334</v>
       </c>
-      <c r="E11" s="9" t="n">
+      <c r="F11" s="9" t="n">
         <v>14.4833333333333</v>
       </c>
     </row>
@@ -569,8 +605,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -583,18 +619,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="11" t="n">
         <v>0.259358851574905</v>
@@ -605,10 +641,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="11" t="n">
         <v>0.282463312755747</v>
@@ -619,10 +655,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>0.238791473009854</v>
@@ -633,10 +669,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="11" t="n">
         <v>0.232695431849424</v>
@@ -647,10 +683,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>0.252007572679306</v>
@@ -661,10 +697,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="11" t="n">
         <v>0.233409356440876</v>
@@ -675,10 +711,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" s="11" t="n">
         <v>0.237528646037034</v>
@@ -689,10 +725,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="11" t="n">
         <v>0.24311749042515</v>
@@ -703,10 +739,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>0.248493826289953</v>
@@ -717,10 +753,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="11" t="n">
         <v>0.228010592689705</v>

</xml_diff>